<commit_message>
add new figure.r, plotting heatmap, boxplot and barplot
</commit_message>
<xml_diff>
--- a/map_property.xlsx
+++ b/map_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000weng_lab\data_R\growth_curve\20250420\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E9427A-AF79-496F-8228-5A8AEED80358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3E942E-B1A8-4FFE-8ADE-530746A03A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="82">
   <si>
     <t>row</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -226,18 +226,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DHFR3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DHFR12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HEXIM1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>7SK(1-175)</t>
   </si>
   <si>
@@ -299,23 +287,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DHFR3_N_term</t>
-  </si>
-  <si>
-    <t>DHFR3_C_term</t>
-  </si>
-  <si>
-    <t>DHFR12_C_term</t>
-  </si>
-  <si>
-    <t>DHFR12_N_term</t>
-  </si>
-  <si>
-    <t>RNA7SK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DHFR12_C_term</t>
+    <t>DHFR_12N3N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHFR_12N3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHFR_12C3N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHFR_12C3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RNA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Protein</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHFR_layout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1641,563 +1637,463 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA022B7-5411-4E42-BF81-094A27934136}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.46484375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="G30" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>